<commit_message>
updated real data- fixed jar gltich
</commit_message>
<xml_diff>
--- a/data/real data.xlsx
+++ b/data/real data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lindsay\Dropbox\Raccoon\larvae\oyster\larvae survival stats\GitHub\RacoonOlyLarvalSurvival\data\RaccoonLikelyhoodLarvaeInJar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lindsay\Dropbox\Raccoon\larvae\oyster\larvae survival stats\GitHub\RacoonOlyLarvalSurvival\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE389450-B252-459F-9CFC-D5815F1528D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8BFA4B-3E3E-4BEC-B2F6-1D195E5B279D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9BF2BB65-623F-4B0F-A177-173AEA287439}"/>
   </bookViews>
@@ -449,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544B3E88-730D-4C30-8A6A-C2D30027C2A2}">
   <dimension ref="A1:H289"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A276" workbookViewId="0">
+      <selection activeCell="K287" sqref="K286:K287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -604,7 +604,7 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -621,7 +621,7 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -638,7 +638,7 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <v>14</v>
@@ -655,7 +655,7 @@
         <v>7</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -672,7 +672,7 @@
         <v>7</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>4</v>
@@ -689,7 +689,7 @@
         <v>7</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14">
         <v>7</v>
@@ -706,7 +706,7 @@
         <v>7</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D15">
         <v>10</v>
@@ -723,7 +723,7 @@
         <v>7</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D16">
         <v>14</v>
@@ -740,7 +740,7 @@
         <v>7</v>
       </c>
       <c r="C17">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -757,7 +757,7 @@
         <v>7</v>
       </c>
       <c r="C18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D18">
         <v>4</v>
@@ -774,7 +774,7 @@
         <v>7</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D19">
         <v>7</v>
@@ -791,7 +791,7 @@
         <v>7</v>
       </c>
       <c r="C20">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D20">
         <v>10</v>
@@ -808,7 +808,7 @@
         <v>7</v>
       </c>
       <c r="C21">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D21">
         <v>14</v>
@@ -825,7 +825,7 @@
         <v>7</v>
       </c>
       <c r="C22">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -842,7 +842,7 @@
         <v>7</v>
       </c>
       <c r="C23">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D23">
         <v>4</v>
@@ -859,7 +859,7 @@
         <v>7</v>
       </c>
       <c r="C24">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D24">
         <v>7</v>
@@ -876,7 +876,7 @@
         <v>7</v>
       </c>
       <c r="C25">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D25">
         <v>10</v>
@@ -893,7 +893,7 @@
         <v>7</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D26">
         <v>14</v>
@@ -910,7 +910,7 @@
         <v>7</v>
       </c>
       <c r="C27">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -927,7 +927,7 @@
         <v>7</v>
       </c>
       <c r="C28">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D28">
         <v>4</v>
@@ -944,7 +944,7 @@
         <v>7</v>
       </c>
       <c r="C29">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D29">
         <v>7</v>
@@ -961,7 +961,7 @@
         <v>7</v>
       </c>
       <c r="C30">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D30">
         <v>10</v>
@@ -978,7 +978,7 @@
         <v>7</v>
       </c>
       <c r="C31">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D31">
         <v>14</v>
@@ -995,7 +995,7 @@
         <v>7</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1012,7 +1012,7 @@
         <v>7</v>
       </c>
       <c r="C33">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D33">
         <v>4</v>
@@ -1029,7 +1029,7 @@
         <v>7</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D34">
         <v>7</v>
@@ -1046,7 +1046,7 @@
         <v>7</v>
       </c>
       <c r="C35">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D35">
         <v>10</v>
@@ -1063,7 +1063,7 @@
         <v>7</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D36">
         <v>14</v>
@@ -1080,7 +1080,7 @@
         <v>7</v>
       </c>
       <c r="C37">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1097,7 +1097,7 @@
         <v>7</v>
       </c>
       <c r="C38">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D38">
         <v>4</v>
@@ -1114,7 +1114,7 @@
         <v>7</v>
       </c>
       <c r="C39">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D39">
         <v>7</v>
@@ -1131,7 +1131,7 @@
         <v>7</v>
       </c>
       <c r="C40">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D40">
         <v>10</v>
@@ -1148,7 +1148,7 @@
         <v>7</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D41">
         <v>14</v>
@@ -1165,7 +1165,7 @@
         <v>7</v>
       </c>
       <c r="C42">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -1182,7 +1182,7 @@
         <v>7</v>
       </c>
       <c r="C43">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D43">
         <v>4</v>
@@ -1199,7 +1199,7 @@
         <v>7</v>
       </c>
       <c r="C44">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D44">
         <v>7</v>
@@ -1216,7 +1216,7 @@
         <v>7</v>
       </c>
       <c r="C45">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D45">
         <v>10</v>
@@ -1233,7 +1233,7 @@
         <v>7</v>
       </c>
       <c r="C46">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D46">
         <v>14</v>
@@ -1250,7 +1250,7 @@
         <v>7</v>
       </c>
       <c r="C47">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -1267,7 +1267,7 @@
         <v>7</v>
       </c>
       <c r="C48">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D48">
         <v>4</v>
@@ -1284,7 +1284,7 @@
         <v>7</v>
       </c>
       <c r="C49">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D49">
         <v>7</v>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="C50">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D50">
         <v>10</v>
@@ -1318,7 +1318,7 @@
         <v>7</v>
       </c>
       <c r="C51">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D51">
         <v>14</v>
@@ -1335,7 +1335,7 @@
         <v>7</v>
       </c>
       <c r="C52">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -1352,7 +1352,7 @@
         <v>7</v>
       </c>
       <c r="C53">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D53">
         <v>4</v>
@@ -1369,7 +1369,7 @@
         <v>7</v>
       </c>
       <c r="C54">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D54">
         <v>7</v>
@@ -1386,7 +1386,7 @@
         <v>7</v>
       </c>
       <c r="C55">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D55">
         <v>10</v>
@@ -1403,7 +1403,7 @@
         <v>7</v>
       </c>
       <c r="C56">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D56">
         <v>14</v>
@@ -1420,7 +1420,7 @@
         <v>7</v>
       </c>
       <c r="C57">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -1437,7 +1437,7 @@
         <v>7</v>
       </c>
       <c r="C58">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D58">
         <v>4</v>
@@ -1454,7 +1454,7 @@
         <v>7</v>
       </c>
       <c r="C59">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D59">
         <v>7</v>
@@ -1471,7 +1471,7 @@
         <v>7</v>
       </c>
       <c r="C60">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D60">
         <v>10</v>
@@ -1488,7 +1488,7 @@
         <v>7</v>
       </c>
       <c r="C61">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D61">
         <v>14</v>
@@ -1505,7 +1505,7 @@
         <v>9</v>
       </c>
       <c r="C62">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -1522,7 +1522,7 @@
         <v>9</v>
       </c>
       <c r="C63">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D63">
         <v>3</v>
@@ -1539,7 +1539,7 @@
         <v>9</v>
       </c>
       <c r="C64">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D64">
         <v>6</v>
@@ -1556,7 +1556,7 @@
         <v>9</v>
       </c>
       <c r="C65">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D65">
         <v>9</v>
@@ -1573,7 +1573,7 @@
         <v>9</v>
       </c>
       <c r="C66">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D66">
         <v>11</v>
@@ -1590,7 +1590,7 @@
         <v>9</v>
       </c>
       <c r="C67">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D67">
         <v>14</v>
@@ -1607,7 +1607,7 @@
         <v>9</v>
       </c>
       <c r="C68">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -1624,7 +1624,7 @@
         <v>9</v>
       </c>
       <c r="C69">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D69">
         <v>3</v>
@@ -1641,7 +1641,7 @@
         <v>9</v>
       </c>
       <c r="C70">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D70">
         <v>6</v>
@@ -1658,7 +1658,7 @@
         <v>9</v>
       </c>
       <c r="C71">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D71">
         <v>9</v>
@@ -1675,7 +1675,7 @@
         <v>9</v>
       </c>
       <c r="C72">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D72">
         <v>11</v>
@@ -1692,7 +1692,7 @@
         <v>9</v>
       </c>
       <c r="C73">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D73">
         <v>14</v>
@@ -1811,7 +1811,7 @@
         <v>9</v>
       </c>
       <c r="C80">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -1828,7 +1828,7 @@
         <v>9</v>
       </c>
       <c r="C81">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D81">
         <v>3</v>
@@ -1845,7 +1845,7 @@
         <v>9</v>
       </c>
       <c r="C82">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D82">
         <v>6</v>
@@ -1862,7 +1862,7 @@
         <v>9</v>
       </c>
       <c r="C83">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D83">
         <v>9</v>
@@ -1879,7 +1879,7 @@
         <v>9</v>
       </c>
       <c r="C84">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D84">
         <v>11</v>
@@ -1896,7 +1896,7 @@
         <v>9</v>
       </c>
       <c r="C85">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D85">
         <v>14</v>
@@ -1913,7 +1913,7 @@
         <v>9</v>
       </c>
       <c r="C86">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -1930,7 +1930,7 @@
         <v>9</v>
       </c>
       <c r="C87">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D87">
         <v>3</v>
@@ -1947,7 +1947,7 @@
         <v>9</v>
       </c>
       <c r="C88">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D88">
         <v>6</v>
@@ -1964,7 +1964,7 @@
         <v>9</v>
       </c>
       <c r="C89">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D89">
         <v>9</v>
@@ -1981,7 +1981,7 @@
         <v>9</v>
       </c>
       <c r="C90">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D90">
         <v>11</v>
@@ -1998,7 +1998,7 @@
         <v>9</v>
       </c>
       <c r="C91">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D91">
         <v>14</v>
@@ -2015,7 +2015,7 @@
         <v>9</v>
       </c>
       <c r="C92">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -2032,7 +2032,7 @@
         <v>9</v>
       </c>
       <c r="C93">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D93">
         <v>3</v>
@@ -2049,7 +2049,7 @@
         <v>9</v>
       </c>
       <c r="C94">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D94">
         <v>6</v>
@@ -2066,7 +2066,7 @@
         <v>9</v>
       </c>
       <c r="C95">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D95">
         <v>9</v>
@@ -2083,7 +2083,7 @@
         <v>9</v>
       </c>
       <c r="C96">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D96">
         <v>11</v>
@@ -2100,7 +2100,7 @@
         <v>9</v>
       </c>
       <c r="C97">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D97">
         <v>14</v>
@@ -2117,7 +2117,7 @@
         <v>9</v>
       </c>
       <c r="C98">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D98">
         <v>1</v>
@@ -2134,7 +2134,7 @@
         <v>9</v>
       </c>
       <c r="C99">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D99">
         <v>3</v>
@@ -2151,7 +2151,7 @@
         <v>9</v>
       </c>
       <c r="C100">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D100">
         <v>6</v>
@@ -2168,7 +2168,7 @@
         <v>9</v>
       </c>
       <c r="C101">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D101">
         <v>9</v>
@@ -2185,7 +2185,7 @@
         <v>9</v>
       </c>
       <c r="C102">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D102">
         <v>11</v>
@@ -2202,7 +2202,7 @@
         <v>9</v>
       </c>
       <c r="C103">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D103">
         <v>14</v>
@@ -2219,7 +2219,7 @@
         <v>9</v>
       </c>
       <c r="C104">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D104">
         <v>1</v>
@@ -2236,7 +2236,7 @@
         <v>9</v>
       </c>
       <c r="C105">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D105">
         <v>3</v>
@@ -2253,7 +2253,7 @@
         <v>9</v>
       </c>
       <c r="C106">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D106">
         <v>6</v>
@@ -2270,7 +2270,7 @@
         <v>9</v>
       </c>
       <c r="C107">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D107">
         <v>9</v>
@@ -2287,7 +2287,7 @@
         <v>9</v>
       </c>
       <c r="C108">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D108">
         <v>11</v>
@@ -2304,7 +2304,7 @@
         <v>9</v>
       </c>
       <c r="C109">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D109">
         <v>14</v>
@@ -2321,7 +2321,7 @@
         <v>9</v>
       </c>
       <c r="C110">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D110">
         <v>1</v>
@@ -2338,7 +2338,7 @@
         <v>9</v>
       </c>
       <c r="C111">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D111">
         <v>3</v>
@@ -2355,7 +2355,7 @@
         <v>9</v>
       </c>
       <c r="C112">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D112">
         <v>6</v>
@@ -2372,7 +2372,7 @@
         <v>9</v>
       </c>
       <c r="C113">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D113">
         <v>9</v>
@@ -2389,7 +2389,7 @@
         <v>9</v>
       </c>
       <c r="C114">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D114">
         <v>11</v>
@@ -2406,7 +2406,7 @@
         <v>9</v>
       </c>
       <c r="C115">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D115">
         <v>14</v>
@@ -2423,7 +2423,7 @@
         <v>9</v>
       </c>
       <c r="C116">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D116">
         <v>1</v>
@@ -2440,7 +2440,7 @@
         <v>9</v>
       </c>
       <c r="C117">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D117">
         <v>3</v>
@@ -2457,7 +2457,7 @@
         <v>9</v>
       </c>
       <c r="C118">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D118">
         <v>6</v>
@@ -2474,7 +2474,7 @@
         <v>9</v>
       </c>
       <c r="C119">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D119">
         <v>9</v>
@@ -2491,7 +2491,7 @@
         <v>9</v>
       </c>
       <c r="C120">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D120">
         <v>11</v>
@@ -2508,7 +2508,7 @@
         <v>9</v>
       </c>
       <c r="C121">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D121">
         <v>14</v>
@@ -2525,7 +2525,7 @@
         <v>9</v>
       </c>
       <c r="C122">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D122">
         <v>1</v>
@@ -2542,7 +2542,7 @@
         <v>9</v>
       </c>
       <c r="C123">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D123">
         <v>3</v>
@@ -2559,7 +2559,7 @@
         <v>9</v>
       </c>
       <c r="C124">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D124">
         <v>6</v>
@@ -2576,7 +2576,7 @@
         <v>9</v>
       </c>
       <c r="C125">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D125">
         <v>9</v>
@@ -2593,7 +2593,7 @@
         <v>9</v>
       </c>
       <c r="C126">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D126">
         <v>11</v>
@@ -2610,7 +2610,7 @@
         <v>9</v>
       </c>
       <c r="C127">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D127">
         <v>14</v>
@@ -2627,7 +2627,7 @@
         <v>9</v>
       </c>
       <c r="C128">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D128">
         <v>1</v>
@@ -2644,7 +2644,7 @@
         <v>9</v>
       </c>
       <c r="C129">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D129">
         <v>3</v>
@@ -2661,7 +2661,7 @@
         <v>9</v>
       </c>
       <c r="C130">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D130">
         <v>6</v>
@@ -2678,7 +2678,7 @@
         <v>9</v>
       </c>
       <c r="C131">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D131">
         <v>9</v>
@@ -2695,7 +2695,7 @@
         <v>9</v>
       </c>
       <c r="C132">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D132">
         <v>11</v>
@@ -2712,7 +2712,7 @@
         <v>9</v>
       </c>
       <c r="C133">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D133">
         <v>14</v>
@@ -2729,7 +2729,7 @@
         <v>10</v>
       </c>
       <c r="C134">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D134">
         <v>1</v>
@@ -2746,7 +2746,7 @@
         <v>10</v>
       </c>
       <c r="C135">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D135">
         <v>3</v>
@@ -2763,7 +2763,7 @@
         <v>10</v>
       </c>
       <c r="C136">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D136">
         <v>5</v>
@@ -2780,7 +2780,7 @@
         <v>10</v>
       </c>
       <c r="C137">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D137">
         <v>7</v>
@@ -2797,7 +2797,7 @@
         <v>10</v>
       </c>
       <c r="C138">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D138">
         <v>10</v>
@@ -2814,7 +2814,7 @@
         <v>10</v>
       </c>
       <c r="C139">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D139">
         <v>12</v>
@@ -2831,7 +2831,7 @@
         <v>10</v>
       </c>
       <c r="C140">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D140">
         <v>14</v>
@@ -2848,7 +2848,7 @@
         <v>10</v>
       </c>
       <c r="C141">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D141">
         <v>1</v>
@@ -2865,7 +2865,7 @@
         <v>10</v>
       </c>
       <c r="C142">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D142">
         <v>3</v>
@@ -2882,7 +2882,7 @@
         <v>10</v>
       </c>
       <c r="C143">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D143">
         <v>5</v>
@@ -2899,7 +2899,7 @@
         <v>10</v>
       </c>
       <c r="C144">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D144">
         <v>7</v>
@@ -3001,7 +3001,7 @@
         <v>10</v>
       </c>
       <c r="C150">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D150">
         <v>5</v>
@@ -3018,7 +3018,7 @@
         <v>10</v>
       </c>
       <c r="C151">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D151">
         <v>7</v>
@@ -3035,7 +3035,7 @@
         <v>10</v>
       </c>
       <c r="C152">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D152">
         <v>10</v>
@@ -3052,7 +3052,7 @@
         <v>10</v>
       </c>
       <c r="C153">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D153">
         <v>12</v>
@@ -3069,7 +3069,7 @@
         <v>10</v>
       </c>
       <c r="C154">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D154">
         <v>14</v>
@@ -3086,7 +3086,7 @@
         <v>10</v>
       </c>
       <c r="C155">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D155">
         <v>1</v>
@@ -3103,7 +3103,7 @@
         <v>10</v>
       </c>
       <c r="C156">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D156">
         <v>3</v>
@@ -3120,7 +3120,7 @@
         <v>10</v>
       </c>
       <c r="C157">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D157">
         <v>5</v>
@@ -3137,7 +3137,7 @@
         <v>10</v>
       </c>
       <c r="C158">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D158">
         <v>7</v>
@@ -3154,7 +3154,7 @@
         <v>10</v>
       </c>
       <c r="C159">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D159">
         <v>10</v>
@@ -3171,7 +3171,7 @@
         <v>10</v>
       </c>
       <c r="C160">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D160">
         <v>12</v>
@@ -3188,7 +3188,7 @@
         <v>10</v>
       </c>
       <c r="C161">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D161">
         <v>14</v>
@@ -3205,7 +3205,7 @@
         <v>10</v>
       </c>
       <c r="C162">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D162">
         <v>1</v>
@@ -3222,7 +3222,7 @@
         <v>10</v>
       </c>
       <c r="C163">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D163">
         <v>3</v>
@@ -3239,7 +3239,7 @@
         <v>10</v>
       </c>
       <c r="C164">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D164">
         <v>5</v>
@@ -3256,7 +3256,7 @@
         <v>10</v>
       </c>
       <c r="C165">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D165">
         <v>7</v>
@@ -3273,7 +3273,7 @@
         <v>10</v>
       </c>
       <c r="C166">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D166">
         <v>10</v>
@@ -3290,7 +3290,7 @@
         <v>10</v>
       </c>
       <c r="C167">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D167">
         <v>12</v>
@@ -3307,7 +3307,7 @@
         <v>10</v>
       </c>
       <c r="C168">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D168">
         <v>14</v>
@@ -3324,7 +3324,7 @@
         <v>10</v>
       </c>
       <c r="C169">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D169">
         <v>1</v>
@@ -3341,7 +3341,7 @@
         <v>10</v>
       </c>
       <c r="C170">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D170">
         <v>3</v>
@@ -3358,7 +3358,7 @@
         <v>10</v>
       </c>
       <c r="C171">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D171">
         <v>5</v>
@@ -3375,7 +3375,7 @@
         <v>10</v>
       </c>
       <c r="C172">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D172">
         <v>7</v>
@@ -3392,7 +3392,7 @@
         <v>10</v>
       </c>
       <c r="C173">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D173">
         <v>10</v>
@@ -3409,7 +3409,7 @@
         <v>10</v>
       </c>
       <c r="C174">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D174">
         <v>12</v>
@@ -3426,7 +3426,7 @@
         <v>10</v>
       </c>
       <c r="C175">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D175">
         <v>14</v>
@@ -3443,7 +3443,7 @@
         <v>10</v>
       </c>
       <c r="C176">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D176">
         <v>1</v>
@@ -3460,7 +3460,7 @@
         <v>10</v>
       </c>
       <c r="C177">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D177">
         <v>3</v>
@@ -3477,7 +3477,7 @@
         <v>10</v>
       </c>
       <c r="C178">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D178">
         <v>5</v>
@@ -3494,7 +3494,7 @@
         <v>10</v>
       </c>
       <c r="C179">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D179">
         <v>7</v>
@@ -3511,7 +3511,7 @@
         <v>10</v>
       </c>
       <c r="C180">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D180">
         <v>10</v>
@@ -3528,7 +3528,7 @@
         <v>10</v>
       </c>
       <c r="C181">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D181">
         <v>12</v>
@@ -3545,7 +3545,7 @@
         <v>10</v>
       </c>
       <c r="C182">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D182">
         <v>14</v>
@@ -3562,7 +3562,7 @@
         <v>10</v>
       </c>
       <c r="C183">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D183">
         <v>1</v>
@@ -3579,7 +3579,7 @@
         <v>10</v>
       </c>
       <c r="C184">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D184">
         <v>3</v>
@@ -3596,7 +3596,7 @@
         <v>10</v>
       </c>
       <c r="C185">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D185">
         <v>5</v>
@@ -3613,7 +3613,7 @@
         <v>10</v>
       </c>
       <c r="C186">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D186">
         <v>7</v>
@@ -3630,7 +3630,7 @@
         <v>10</v>
       </c>
       <c r="C187">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D187">
         <v>10</v>
@@ -3647,7 +3647,7 @@
         <v>10</v>
       </c>
       <c r="C188">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D188">
         <v>12</v>
@@ -3664,7 +3664,7 @@
         <v>10</v>
       </c>
       <c r="C189">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D189">
         <v>14</v>
@@ -3681,7 +3681,7 @@
         <v>10</v>
       </c>
       <c r="C190">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D190">
         <v>1</v>
@@ -3698,7 +3698,7 @@
         <v>10</v>
       </c>
       <c r="C191">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D191">
         <v>3</v>
@@ -3715,7 +3715,7 @@
         <v>10</v>
       </c>
       <c r="C192">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D192">
         <v>5</v>
@@ -3732,7 +3732,7 @@
         <v>10</v>
       </c>
       <c r="C193">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D193">
         <v>7</v>
@@ -3749,7 +3749,7 @@
         <v>10</v>
       </c>
       <c r="C194">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D194">
         <v>10</v>
@@ -3766,7 +3766,7 @@
         <v>10</v>
       </c>
       <c r="C195">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D195">
         <v>12</v>
@@ -3783,7 +3783,7 @@
         <v>10</v>
       </c>
       <c r="C196">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D196">
         <v>14</v>
@@ -3800,7 +3800,7 @@
         <v>10</v>
       </c>
       <c r="C197">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D197">
         <v>1</v>
@@ -3817,7 +3817,7 @@
         <v>10</v>
       </c>
       <c r="C198">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D198">
         <v>3</v>
@@ -3834,7 +3834,7 @@
         <v>10</v>
       </c>
       <c r="C199">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D199">
         <v>5</v>
@@ -3851,7 +3851,7 @@
         <v>10</v>
       </c>
       <c r="C200">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D200">
         <v>7</v>
@@ -3868,7 +3868,7 @@
         <v>10</v>
       </c>
       <c r="C201">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D201">
         <v>10</v>
@@ -3885,7 +3885,7 @@
         <v>10</v>
       </c>
       <c r="C202">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D202">
         <v>12</v>
@@ -3902,7 +3902,7 @@
         <v>10</v>
       </c>
       <c r="C203">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D203">
         <v>14</v>
@@ -3919,7 +3919,7 @@
         <v>10</v>
       </c>
       <c r="C204">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D204">
         <v>1</v>
@@ -3936,7 +3936,7 @@
         <v>10</v>
       </c>
       <c r="C205">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D205">
         <v>3</v>
@@ -3953,7 +3953,7 @@
         <v>10</v>
       </c>
       <c r="C206">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D206">
         <v>5</v>
@@ -3970,7 +3970,7 @@
         <v>10</v>
       </c>
       <c r="C207">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D207">
         <v>7</v>
@@ -3987,7 +3987,7 @@
         <v>10</v>
       </c>
       <c r="C208">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D208">
         <v>10</v>
@@ -4004,7 +4004,7 @@
         <v>10</v>
       </c>
       <c r="C209">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D209">
         <v>12</v>
@@ -4021,7 +4021,7 @@
         <v>10</v>
       </c>
       <c r="C210">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D210">
         <v>14</v>
@@ -4038,7 +4038,7 @@
         <v>10</v>
       </c>
       <c r="C211">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D211">
         <v>1</v>
@@ -4259,7 +4259,7 @@
         <v>11</v>
       </c>
       <c r="C224">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D224">
         <v>1</v>
@@ -4276,7 +4276,7 @@
         <v>11</v>
       </c>
       <c r="C225">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D225">
         <v>4</v>
@@ -4293,7 +4293,7 @@
         <v>11</v>
       </c>
       <c r="C226">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D226">
         <v>7</v>
@@ -4310,7 +4310,7 @@
         <v>11</v>
       </c>
       <c r="C227">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D227">
         <v>10</v>
@@ -4327,7 +4327,7 @@
         <v>11</v>
       </c>
       <c r="C228">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D228">
         <v>12</v>
@@ -4344,7 +4344,7 @@
         <v>11</v>
       </c>
       <c r="C229">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D229">
         <v>14</v>
@@ -4361,7 +4361,7 @@
         <v>11</v>
       </c>
       <c r="C230">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D230">
         <v>1</v>
@@ -4378,7 +4378,7 @@
         <v>11</v>
       </c>
       <c r="C231">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D231">
         <v>4</v>
@@ -4395,7 +4395,7 @@
         <v>11</v>
       </c>
       <c r="C232">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D232">
         <v>7</v>
@@ -4412,7 +4412,7 @@
         <v>11</v>
       </c>
       <c r="C233">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D233">
         <v>10</v>
@@ -4429,7 +4429,7 @@
         <v>11</v>
       </c>
       <c r="C234">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D234">
         <v>12</v>
@@ -4446,7 +4446,7 @@
         <v>11</v>
       </c>
       <c r="C235">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D235">
         <v>14</v>
@@ -4463,7 +4463,7 @@
         <v>11</v>
       </c>
       <c r="C236">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D236">
         <v>1</v>
@@ -4480,7 +4480,7 @@
         <v>11</v>
       </c>
       <c r="C237">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D237">
         <v>4</v>
@@ -4497,7 +4497,7 @@
         <v>11</v>
       </c>
       <c r="C238">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D238">
         <v>7</v>
@@ -4514,7 +4514,7 @@
         <v>11</v>
       </c>
       <c r="C239">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D239">
         <v>10</v>
@@ -4531,7 +4531,7 @@
         <v>11</v>
       </c>
       <c r="C240">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D240">
         <v>12</v>
@@ -4548,7 +4548,7 @@
         <v>11</v>
       </c>
       <c r="C241">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D241">
         <v>14</v>
@@ -4565,7 +4565,7 @@
         <v>11</v>
       </c>
       <c r="C242">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D242">
         <v>1</v>
@@ -4582,7 +4582,7 @@
         <v>11</v>
       </c>
       <c r="C243">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D243">
         <v>4</v>
@@ -4599,7 +4599,7 @@
         <v>11</v>
       </c>
       <c r="C244">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D244">
         <v>7</v>
@@ -4616,7 +4616,7 @@
         <v>11</v>
       </c>
       <c r="C245">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D245">
         <v>10</v>
@@ -4633,7 +4633,7 @@
         <v>11</v>
       </c>
       <c r="C246">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D246">
         <v>12</v>
@@ -4650,7 +4650,7 @@
         <v>11</v>
       </c>
       <c r="C247">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D247">
         <v>14</v>
@@ -4667,7 +4667,7 @@
         <v>11</v>
       </c>
       <c r="C248">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D248">
         <v>1</v>
@@ -4684,7 +4684,7 @@
         <v>11</v>
       </c>
       <c r="C249">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D249">
         <v>4</v>
@@ -4701,7 +4701,7 @@
         <v>11</v>
       </c>
       <c r="C250">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D250">
         <v>7</v>
@@ -4718,7 +4718,7 @@
         <v>11</v>
       </c>
       <c r="C251">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D251">
         <v>10</v>
@@ -4735,7 +4735,7 @@
         <v>11</v>
       </c>
       <c r="C252">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D252">
         <v>12</v>
@@ -4752,7 +4752,7 @@
         <v>11</v>
       </c>
       <c r="C253">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D253">
         <v>14</v>
@@ -4769,7 +4769,7 @@
         <v>11</v>
       </c>
       <c r="C254">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D254">
         <v>1</v>
@@ -4786,7 +4786,7 @@
         <v>11</v>
       </c>
       <c r="C255">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D255">
         <v>4</v>
@@ -4803,7 +4803,7 @@
         <v>11</v>
       </c>
       <c r="C256">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D256">
         <v>7</v>
@@ -4820,7 +4820,7 @@
         <v>11</v>
       </c>
       <c r="C257">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D257">
         <v>10</v>
@@ -4837,7 +4837,7 @@
         <v>11</v>
       </c>
       <c r="C258">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D258">
         <v>12</v>
@@ -4854,7 +4854,7 @@
         <v>11</v>
       </c>
       <c r="C259">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D259">
         <v>14</v>
@@ -4871,7 +4871,7 @@
         <v>11</v>
       </c>
       <c r="C260">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D260">
         <v>1</v>
@@ -4888,7 +4888,7 @@
         <v>11</v>
       </c>
       <c r="C261">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D261">
         <v>4</v>
@@ -4905,7 +4905,7 @@
         <v>11</v>
       </c>
       <c r="C262">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D262">
         <v>7</v>
@@ -4922,7 +4922,7 @@
         <v>11</v>
       </c>
       <c r="C263">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D263">
         <v>10</v>
@@ -4939,7 +4939,7 @@
         <v>11</v>
       </c>
       <c r="C264">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D264">
         <v>12</v>
@@ -4956,7 +4956,7 @@
         <v>11</v>
       </c>
       <c r="C265">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D265">
         <v>14</v>
@@ -4973,7 +4973,7 @@
         <v>11</v>
       </c>
       <c r="C266">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D266">
         <v>1</v>
@@ -4990,7 +4990,7 @@
         <v>11</v>
       </c>
       <c r="C267">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D267">
         <v>4</v>
@@ -5007,7 +5007,7 @@
         <v>11</v>
       </c>
       <c r="C268">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D268">
         <v>7</v>
@@ -5024,7 +5024,7 @@
         <v>11</v>
       </c>
       <c r="C269">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D269">
         <v>10</v>
@@ -5041,7 +5041,7 @@
         <v>11</v>
       </c>
       <c r="C270">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D270">
         <v>12</v>
@@ -5058,7 +5058,7 @@
         <v>11</v>
       </c>
       <c r="C271">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D271">
         <v>14</v>
@@ -5075,7 +5075,7 @@
         <v>11</v>
       </c>
       <c r="C272">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D272">
         <v>1</v>
@@ -5092,7 +5092,7 @@
         <v>11</v>
       </c>
       <c r="C273">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D273">
         <v>4</v>
@@ -5109,7 +5109,7 @@
         <v>11</v>
       </c>
       <c r="C274">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D274">
         <v>7</v>
@@ -5126,7 +5126,7 @@
         <v>11</v>
       </c>
       <c r="C275">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D275">
         <v>10</v>
@@ -5143,7 +5143,7 @@
         <v>11</v>
       </c>
       <c r="C276">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D276">
         <v>12</v>
@@ -5160,7 +5160,7 @@
         <v>11</v>
       </c>
       <c r="C277">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D277">
         <v>14</v>
@@ -5177,7 +5177,7 @@
         <v>11</v>
       </c>
       <c r="C278">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D278">
         <v>1</v>
@@ -5194,7 +5194,7 @@
         <v>11</v>
       </c>
       <c r="C279">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D279">
         <v>4</v>
@@ -5211,7 +5211,7 @@
         <v>11</v>
       </c>
       <c r="C280">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D280">
         <v>7</v>
@@ -5228,7 +5228,7 @@
         <v>11</v>
       </c>
       <c r="C281">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D281">
         <v>10</v>
@@ -5245,7 +5245,7 @@
         <v>11</v>
       </c>
       <c r="C282">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D282">
         <v>12</v>
@@ -5262,7 +5262,7 @@
         <v>11</v>
       </c>
       <c r="C283">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D283">
         <v>14</v>

</xml_diff>